<commit_message>
modified template report, change to use Regular expressions when input option params Add test case, add new blog
</commit_message>
<xml_diff>
--- a/src/test/java/pHpFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/pHpFox/testdata/v5DataProvider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\pHpFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56000B9-56AB-4ABD-B0A3-CC65D6001911}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8870986-9A8E-4C41-AA49-4AF224E1ACF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="160">
   <si>
     <t>id</t>
   </si>
@@ -642,6 +642,12 @@
   </si>
   <si>
     <t>The user credentials were incorrect.</t>
+  </si>
+  <si>
+    <t>blogs</t>
+  </si>
+  <si>
+    <t>photos</t>
   </si>
 </sst>
 </file>
@@ -701,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -717,6 +723,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,7 +1048,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1153,7 +1162,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>21</v>
@@ -1175,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
@@ -1186,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
@@ -1208,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>26</v>
@@ -1219,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>27</v>
@@ -1230,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>28</v>
@@ -1549,7 +1558,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>60</v>
@@ -1560,7 +1569,7 @@
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>60</v>
@@ -1571,7 +1580,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>61</v>
@@ -1604,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>64</v>
@@ -1615,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>65</v>
@@ -1637,7 +1646,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>67</v>
@@ -1648,7 +1657,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>68</v>
@@ -1659,7 +1668,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>69</v>
@@ -1670,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>70</v>
@@ -2285,7 +2294,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2357,7 +2366,7 @@
       <c r="E2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>138</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -2377,7 +2386,7 @@
       <c r="E3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <v>123456</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -2397,7 +2406,7 @@
       <c r="E4" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="9">
         <v>123456</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -2417,7 +2426,7 @@
       <c r="E5" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="9">
         <v>123456</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -2437,7 +2446,7 @@
       <c r="E6" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="9">
         <v>123456</v>
       </c>
       <c r="G6" s="3" t="s">

</xml_diff>

<commit_message>
modified function add new blog, add "search, edit" blog. change flow login many users
</commit_message>
<xml_diff>
--- a/src/test/java/pHpFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/pHpFox/testdata/v5DataProvider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\pHpFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8870986-9A8E-4C41-AA49-4AF224E1ACF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F2484B-860B-4FB2-A262-8C0E30FF41BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="163">
   <si>
     <t>id</t>
   </si>
@@ -236,9 +236,6 @@
     <t>/blog</t>
   </si>
   <si>
-    <t>/blog/1</t>
-  </si>
-  <si>
     <t>/blog/add</t>
   </si>
   <si>
@@ -530,9 +527,6 @@
     <t>/video</t>
   </si>
   <si>
-    <t>/video/1</t>
-  </si>
-  <si>
     <t>/video/add</t>
   </si>
   <si>
@@ -605,9 +599,6 @@
     <t>terry</t>
   </si>
   <si>
-    <t>terry@example.net123456</t>
-  </si>
-  <si>
     <t>/terry</t>
   </si>
   <si>
@@ -648,13 +639,31 @@
   </si>
   <si>
     <t>photos</t>
+  </si>
+  <si>
+    <t>terry@example.net</t>
+  </si>
+  <si>
+    <t>friends</t>
+  </si>
+  <si>
+    <t>videos</t>
+  </si>
+  <si>
+    <t>/video/all</t>
+  </si>
+  <si>
+    <t>/blog/all</t>
+  </si>
+  <si>
+    <t>poll___</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -686,6 +695,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -704,10 +720,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -726,8 +743,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1046,9 +1065,9 @@
   </sheetPr>
   <dimension ref="A1:AC107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>21</v>
@@ -1173,10 +1192,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -1184,10 +1203,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -1195,10 +1214,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -1209,7 +1228,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -1217,10 +1236,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -1228,10 +1247,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -1239,10 +1258,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -1253,7 +1272,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -1264,7 +1283,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -1272,10 +1291,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -1283,10 +1302,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -1294,10 +1313,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -1305,10 +1324,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
@@ -1316,10 +1335,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
@@ -1327,10 +1346,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
@@ -1338,10 +1357,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
@@ -1349,10 +1368,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
@@ -1360,10 +1379,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -1371,10 +1390,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -1382,10 +1401,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -1393,10 +1412,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
@@ -1404,10 +1423,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
@@ -1415,10 +1434,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
@@ -1426,10 +1445,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
@@ -1437,10 +1456,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
@@ -1448,10 +1467,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -1459,10 +1478,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -1470,10 +1489,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -1481,10 +1500,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -1492,10 +1511,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -1503,10 +1522,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -1514,10 +1533,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -1525,10 +1544,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>54</v>
+        <v>158</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -1536,10 +1555,10 @@
         <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -1547,10 +1566,10 @@
         <v>4</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -1558,10 +1577,10 @@
         <v>5</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -1569,10 +1588,10 @@
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -1580,10 +1599,10 @@
         <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -1591,10 +1610,10 @@
         <v>5</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -1602,10 +1621,10 @@
         <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -1613,10 +1632,10 @@
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -1624,10 +1643,10 @@
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -1635,10 +1654,10 @@
         <v>5</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -1646,10 +1665,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
@@ -1657,10 +1676,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -1668,10 +1687,10 @@
         <v>5</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -1679,10 +1698,10 @@
         <v>5</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -1690,10 +1709,10 @@
         <v>6</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
@@ -1701,10 +1720,10 @@
         <v>6</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -1712,10 +1731,10 @@
         <v>6</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>71</v>
+        <v>162</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -1723,10 +1742,10 @@
         <v>6</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
@@ -1734,10 +1753,10 @@
         <v>6</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>71</v>
+        <v>162</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -1745,10 +1764,10 @@
         <v>6</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
@@ -1756,10 +1775,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -1767,10 +1786,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>71</v>
+        <v>162</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
@@ -1778,10 +1797,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>71</v>
+        <v>162</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -1789,10 +1808,10 @@
         <v>7</v>
       </c>
       <c r="C63" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
@@ -1800,10 +1819,10 @@
         <v>7</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
@@ -1811,10 +1830,10 @@
         <v>7</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -1822,10 +1841,10 @@
         <v>7</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
@@ -1833,10 +1852,10 @@
         <v>7</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -1844,10 +1863,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
@@ -1855,10 +1874,10 @@
         <v>7</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
@@ -1866,10 +1885,10 @@
         <v>7</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
@@ -1877,10 +1896,10 @@
         <v>7</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
@@ -1888,10 +1907,10 @@
         <v>7</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
@@ -1899,10 +1918,10 @@
         <v>7</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
@@ -1910,10 +1929,10 @@
         <v>8</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
@@ -1921,10 +1940,10 @@
         <v>8</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
@@ -1932,10 +1951,10 @@
         <v>8</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
@@ -1943,10 +1962,10 @@
         <v>8</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
@@ -1954,10 +1973,10 @@
         <v>8</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
@@ -1965,10 +1984,10 @@
         <v>8</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
@@ -1976,10 +1995,10 @@
         <v>8</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
@@ -1987,10 +2006,10 @@
         <v>8</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
@@ -1998,10 +2017,10 @@
         <v>8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
@@ -2009,10 +2028,10 @@
         <v>8</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
@@ -2020,10 +2039,10 @@
         <v>8</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
@@ -2031,10 +2050,10 @@
         <v>8</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
@@ -2042,10 +2061,10 @@
         <v>8</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -2053,10 +2072,10 @@
         <v>9</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
@@ -2064,10 +2083,10 @@
         <v>9</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
@@ -2075,10 +2094,10 @@
         <v>9</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
@@ -2086,10 +2105,10 @@
         <v>9</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.2">
@@ -2097,10 +2116,10 @@
         <v>9</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.2">
@@ -2108,10 +2127,10 @@
         <v>9</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.2">
@@ -2119,10 +2138,10 @@
         <v>9</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.2">
@@ -2130,10 +2149,10 @@
         <v>9</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.2">
@@ -2141,10 +2160,10 @@
         <v>10</v>
       </c>
       <c r="C95" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
@@ -2152,10 +2171,10 @@
         <v>11</v>
       </c>
       <c r="C96" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.2">
@@ -2163,10 +2182,10 @@
         <v>12</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.2">
@@ -2174,10 +2193,10 @@
         <v>12</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
@@ -2188,7 +2207,7 @@
         <v>9</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
@@ -2199,7 +2218,7 @@
         <v>9</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.2">
@@ -2210,7 +2229,7 @@
         <v>9</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
@@ -2218,10 +2237,10 @@
         <v>12</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
@@ -2229,10 +2248,10 @@
         <v>12</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.2">
@@ -2243,7 +2262,7 @@
         <v>9</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
@@ -2254,7 +2273,7 @@
         <v>9</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.2">
@@ -2265,7 +2284,7 @@
         <v>9</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.2">
@@ -2273,10 +2292,10 @@
         <v>14</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2292,9 +2311,9 @@
   </sheetPr>
   <dimension ref="A1:AC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2303,7 +2322,7 @@
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2315,16 +2334,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -2333,7 +2352,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -2358,102 +2377,102 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="F3" s="9">
         <v>123456</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="F4" s="9">
         <v>123456</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F5" s="9">
         <v>123456</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F6" s="9">
         <v>123456</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -5442,9 +5461,13 @@
       <c r="F1001" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{503540FC-8460-4D96-A4D6-6C87EEBE8A4E}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B1AF28E8-005A-4456-9047-1070A5527857}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -5477,16 +5500,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
re-struct page objects, step defined and scenarios
</commit_message>
<xml_diff>
--- a/src/test/java/pHpFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/pHpFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\pHpFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F2484B-860B-4FB2-A262-8C0E30FF41BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95E2A99-8110-4308-B736-7F3CE3412018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="164">
   <si>
     <t>id</t>
   </si>
@@ -329,9 +329,6 @@
     <t>/forgot-password</t>
   </si>
   <si>
-    <t>friend</t>
-  </si>
-  <si>
     <t>/friend</t>
   </si>
   <si>
@@ -635,12 +632,6 @@
     <t>The user credentials were incorrect.</t>
   </si>
   <si>
-    <t>blogs</t>
-  </si>
-  <si>
-    <t>photos</t>
-  </si>
-  <si>
     <t>terry@example.net</t>
   </si>
   <si>
@@ -657,6 +648,18 @@
   </si>
   <si>
     <t>poll___</t>
+  </si>
+  <si>
+    <t>blog___</t>
+  </si>
+  <si>
+    <t>blog_+_</t>
+  </si>
+  <si>
+    <t>photo_</t>
+  </si>
+  <si>
+    <t>friend_</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1069,8 @@
   <dimension ref="A1:AC107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1181,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>21</v>
@@ -1192,10 +1195,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -1203,7 +1206,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
@@ -1214,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>23</v>
@@ -1225,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -1236,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>25</v>
@@ -1247,7 +1250,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>26</v>
@@ -1258,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>27</v>
@@ -1269,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>20</v>
+        <v>161</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>28</v>
@@ -1280,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>29</v>
@@ -1533,10 +1536,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -1544,10 +1547,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -1555,10 +1558,10 @@
         <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -1566,10 +1569,10 @@
         <v>4</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -1577,10 +1580,10 @@
         <v>5</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -1588,10 +1591,10 @@
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -1599,10 +1602,10 @@
         <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -1610,10 +1613,10 @@
         <v>5</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -1621,10 +1624,10 @@
         <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -1632,10 +1635,10 @@
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -1643,10 +1646,10 @@
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -1654,10 +1657,10 @@
         <v>5</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -1665,10 +1668,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
@@ -1676,10 +1679,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -1687,10 +1690,10 @@
         <v>5</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -1698,10 +1701,10 @@
         <v>5</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -1709,10 +1712,10 @@
         <v>6</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
@@ -1720,10 +1723,10 @@
         <v>6</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -1731,10 +1734,10 @@
         <v>6</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -1742,10 +1745,10 @@
         <v>6</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
@@ -1753,10 +1756,10 @@
         <v>6</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -1764,10 +1767,10 @@
         <v>6</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
@@ -1775,10 +1778,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -1786,10 +1789,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
@@ -1797,10 +1800,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -1808,10 +1811,10 @@
         <v>7</v>
       </c>
       <c r="C63" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
@@ -1819,10 +1822,10 @@
         <v>7</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
@@ -1830,10 +1833,10 @@
         <v>7</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -1841,10 +1844,10 @@
         <v>7</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
@@ -1852,10 +1855,10 @@
         <v>7</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -1863,10 +1866,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
@@ -1874,10 +1877,10 @@
         <v>7</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
@@ -1885,10 +1888,10 @@
         <v>7</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
@@ -1896,10 +1899,10 @@
         <v>7</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
@@ -1907,10 +1910,10 @@
         <v>7</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
@@ -1918,10 +1921,10 @@
         <v>7</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
@@ -1929,10 +1932,10 @@
         <v>8</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
@@ -1940,10 +1943,10 @@
         <v>8</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
@@ -1951,10 +1954,10 @@
         <v>8</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
@@ -1962,10 +1965,10 @@
         <v>8</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
@@ -1973,10 +1976,10 @@
         <v>8</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
@@ -1984,10 +1987,10 @@
         <v>8</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
@@ -1995,10 +1998,10 @@
         <v>8</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
@@ -2006,10 +2009,10 @@
         <v>8</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
@@ -2017,10 +2020,10 @@
         <v>8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
@@ -2028,10 +2031,10 @@
         <v>8</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
@@ -2039,10 +2042,10 @@
         <v>8</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
@@ -2050,10 +2053,10 @@
         <v>8</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
@@ -2061,10 +2064,10 @@
         <v>8</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -2072,10 +2075,10 @@
         <v>9</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
@@ -2083,10 +2086,10 @@
         <v>9</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
@@ -2094,10 +2097,10 @@
         <v>9</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
@@ -2105,10 +2108,10 @@
         <v>9</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.2">
@@ -2116,10 +2119,10 @@
         <v>9</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.2">
@@ -2127,10 +2130,10 @@
         <v>9</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.2">
@@ -2138,10 +2141,10 @@
         <v>9</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.2">
@@ -2149,10 +2152,10 @@
         <v>9</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.2">
@@ -2160,10 +2163,10 @@
         <v>10</v>
       </c>
       <c r="C95" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
@@ -2171,10 +2174,10 @@
         <v>11</v>
       </c>
       <c r="C96" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.2">
@@ -2182,10 +2185,10 @@
         <v>12</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.2">
@@ -2193,10 +2196,10 @@
         <v>12</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
@@ -2207,7 +2210,7 @@
         <v>9</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
@@ -2218,7 +2221,7 @@
         <v>9</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.2">
@@ -2229,7 +2232,7 @@
         <v>9</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
@@ -2237,10 +2240,10 @@
         <v>12</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
@@ -2248,10 +2251,10 @@
         <v>12</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.2">
@@ -2262,7 +2265,7 @@
         <v>9</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
@@ -2273,7 +2276,7 @@
         <v>9</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.2">
@@ -2284,7 +2287,7 @@
         <v>9</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.2">
@@ -2292,10 +2295,10 @@
         <v>14</v>
       </c>
       <c r="C107" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2316,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2334,16 +2337,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -2352,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -2377,102 +2380,102 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>138</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>139</v>
       </c>
       <c r="F3" s="9">
         <v>123456</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F4" s="9">
         <v>123456</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="F5" s="9">
         <v>123456</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="F6" s="9">
         <v>123456</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -5500,16 +5503,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>

</xml_diff>